<commit_message>
HuyenPT: Update Use Case List
</commit_message>
<xml_diff>
--- a/WIP/Documents/UseCase Diagram/List of UseCase.xlsx
+++ b/WIP/Documents/UseCase Diagram/List of UseCase.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="201">
   <si>
     <t>Use Case No.</t>
   </si>
@@ -537,18 +537,6 @@
     <t>Xóa nhà xuất bản</t>
   </si>
   <si>
-    <t>SYSTEM MODULE</t>
-  </si>
-  <si>
-    <t>Send confirm mail to active an account</t>
-  </si>
-  <si>
-    <t>Gửi mail xác nhận khi người dùng yêu cầu lập tài khoản</t>
-  </si>
-  <si>
-    <t>Gửi mail thông báo mật khẩu mới khi người dùng sử dụng chức năng quên mật khẩu</t>
-  </si>
-  <si>
     <t>UC050</t>
   </si>
   <si>
@@ -561,12 +549,6 @@
     <t>UC053</t>
   </si>
   <si>
-    <t>Statistic access times</t>
-  </si>
-  <si>
-    <t>Statistic</t>
-  </si>
-  <si>
     <t>Decline  request about reporting an account/group</t>
   </si>
   <si>
@@ -576,18 +558,6 @@
     <t>Suggest book/author</t>
   </si>
   <si>
-    <t>Send warning mail to reported user</t>
-  </si>
-  <si>
-    <t>UC054</t>
-  </si>
-  <si>
-    <t>UC055</t>
-  </si>
-  <si>
-    <t>Gửi mail cảnh cáo cho người dùng bị report</t>
-  </si>
-  <si>
     <t>Giới thiệu sách/tác giả cho người dùng: Dựa trên danh sách những sách họ bình chọn, tác giả đang theo dõi</t>
   </si>
   <si>
@@ -603,9 +573,6 @@
     <t>Delete publisher</t>
   </si>
   <si>
-    <t>Send  mail to reset password</t>
-  </si>
-  <si>
     <t>Reset pasword</t>
   </si>
   <si>
@@ -651,41 +618,14 @@
     <t>Xem thông tin thống kê lượt truy cập</t>
   </si>
   <si>
-    <t>Statistic users</t>
-  </si>
-  <si>
-    <t>Statistic authors</t>
-  </si>
-  <si>
-    <t>Statistic groups</t>
-  </si>
-  <si>
-    <t>Statistic books</t>
-  </si>
-  <si>
-    <t>Thống kê về người dùng thường</t>
-  </si>
-  <si>
-    <t>Thống kê về tác giả</t>
-  </si>
-  <si>
-    <t>Thống kê về nhóm</t>
-  </si>
-  <si>
-    <t>Thống kê về sách</t>
-  </si>
-  <si>
-    <t>Thống kê về lượt truy cập</t>
-  </si>
-  <si>
-    <t>Send mail</t>
+    <t>BSN SYSTEM MODULE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -707,14 +647,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -850,7 +782,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -897,32 +829,38 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -936,12 +874,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -950,33 +888,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1279,7 +1190,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D5:G82"/>
+  <dimension ref="D5:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -1307,27 +1218,27 @@
       </c>
     </row>
     <row r="6" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
     </row>
     <row r="7" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
     </row>
     <row r="8" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>198</v>
+      <c r="E8" s="21" t="s">
+        <v>187</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>6</v>
@@ -1337,8 +1248,8 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1347,8 +1258,8 @@
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D10" s="19"/>
-      <c r="E10" s="24"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="22"/>
       <c r="F10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1360,7 +1271,7 @@
       <c r="D11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="19"/>
+      <c r="E11" s="23"/>
       <c r="F11" s="4" t="s">
         <v>13</v>
       </c>
@@ -1369,10 +1280,10 @@
       </c>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="21" t="s">
         <v>17</v>
       </c>
       <c r="F12" s="4" t="s">
@@ -1383,8 +1294,8 @@
       </c>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
       <c r="F13" s="4" t="s">
         <v>131</v>
       </c>
@@ -1410,25 +1321,25 @@
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="4" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="37"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" spans="4:7" ht="45" x14ac:dyDescent="0.25">
       <c r="D17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="21" t="s">
         <v>47</v>
       </c>
       <c r="F17" s="4" t="s">
@@ -1439,10 +1350,10 @@
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="24"/>
+      <c r="E18" s="22"/>
       <c r="F18" s="4" t="s">
         <v>27</v>
       </c>
@@ -1451,8 +1362,8 @@
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="19"/>
-      <c r="E19" s="24"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="22"/>
       <c r="F19" s="4" t="s">
         <v>28</v>
       </c>
@@ -1464,7 +1375,7 @@
       <c r="D20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="24"/>
+      <c r="E20" s="22"/>
       <c r="F20" s="4" t="s">
         <v>31</v>
       </c>
@@ -1476,7 +1387,7 @@
       <c r="D21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="24"/>
+      <c r="E21" s="22"/>
       <c r="F21" s="4" t="s">
         <v>53</v>
       </c>
@@ -1488,7 +1399,7 @@
       <c r="D22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="19"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="4" t="s">
         <v>54</v>
       </c>
@@ -1500,7 +1411,7 @@
       <c r="D23" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="21" t="s">
         <v>48</v>
       </c>
       <c r="F23" s="4" t="s">
@@ -1514,7 +1425,7 @@
       <c r="D24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="24"/>
+      <c r="E24" s="22"/>
       <c r="F24" s="4" t="s">
         <v>42</v>
       </c>
@@ -1526,7 +1437,7 @@
       <c r="D25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="24"/>
+      <c r="E25" s="22"/>
       <c r="F25" s="4" t="s">
         <v>43</v>
       </c>
@@ -1538,7 +1449,7 @@
       <c r="D26" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="19"/>
+      <c r="E26" s="23"/>
       <c r="F26" s="4" t="s">
         <v>34</v>
       </c>
@@ -1550,7 +1461,7 @@
       <c r="D27" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="28" t="s">
+      <c r="E27" s="30" t="s">
         <v>46</v>
       </c>
       <c r="F27" s="4" t="s">
@@ -1564,7 +1475,7 @@
       <c r="D28" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E28" s="30"/>
+      <c r="E28" s="31"/>
       <c r="F28" s="4" t="s">
         <v>44</v>
       </c>
@@ -1576,7 +1487,7 @@
       <c r="D29" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E29" s="30"/>
+      <c r="E29" s="31"/>
       <c r="F29" s="4" t="s">
         <v>45</v>
       </c>
@@ -1588,7 +1499,7 @@
       <c r="D30" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E30" s="29"/>
+      <c r="E30" s="32"/>
       <c r="F30" s="4" t="s">
         <v>35</v>
       </c>
@@ -1597,19 +1508,19 @@
       </c>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="33"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="35"/>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D32" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E32" s="28" t="s">
-        <v>199</v>
+      <c r="E32" s="30" t="s">
+        <v>188</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>65</v>
@@ -1622,7 +1533,7 @@
       <c r="D33" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E33" s="30"/>
+      <c r="E33" s="31"/>
       <c r="F33" s="6" t="s">
         <v>69</v>
       </c>
@@ -1634,7 +1545,7 @@
       <c r="D34" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="29"/>
+      <c r="E34" s="32"/>
       <c r="F34" s="6" t="s">
         <v>115</v>
       </c>
@@ -1646,8 +1557,8 @@
       <c r="D35" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E35" s="18" t="s">
-        <v>200</v>
+      <c r="E35" s="21" t="s">
+        <v>189</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>99</v>
@@ -1660,7 +1571,7 @@
       <c r="D36" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E36" s="24"/>
+      <c r="E36" s="22"/>
       <c r="F36" s="4" t="s">
         <v>100</v>
       </c>
@@ -1672,7 +1583,7 @@
       <c r="D37" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="E37" s="19"/>
+      <c r="E37" s="23"/>
       <c r="F37" s="4" t="s">
         <v>116</v>
       </c>
@@ -1681,19 +1592,19 @@
       </c>
     </row>
     <row r="38" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D38" s="25" t="s">
+      <c r="D38" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="27"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="29"/>
     </row>
     <row r="39" spans="4:7" ht="30" x14ac:dyDescent="0.25">
       <c r="D39" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E39" s="18" t="s">
-        <v>201</v>
+      <c r="E39" s="21" t="s">
+        <v>190</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>72</v>
@@ -1706,7 +1617,7 @@
       <c r="D40" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E40" s="24"/>
+      <c r="E40" s="22"/>
       <c r="F40" s="4" t="s">
         <v>84</v>
       </c>
@@ -1718,7 +1629,7 @@
       <c r="D41" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E41" s="19"/>
+      <c r="E41" s="23"/>
       <c r="F41" s="4" t="s">
         <v>88</v>
       </c>
@@ -1730,7 +1641,7 @@
       <c r="D42" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E42" s="28" t="s">
+      <c r="E42" s="30" t="s">
         <v>119</v>
       </c>
       <c r="F42" s="6" t="s">
@@ -1744,7 +1655,7 @@
       <c r="D43" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E43" s="30"/>
+      <c r="E43" s="31"/>
       <c r="F43" s="6" t="s">
         <v>76</v>
       </c>
@@ -1756,7 +1667,7 @@
       <c r="D44" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E44" s="30"/>
+      <c r="E44" s="31"/>
       <c r="F44" s="4" t="s">
         <v>77</v>
       </c>
@@ -1768,7 +1679,7 @@
       <c r="D45" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E45" s="29"/>
+      <c r="E45" s="32"/>
       <c r="F45" s="4" t="s">
         <v>82</v>
       </c>
@@ -1780,7 +1691,7 @@
       <c r="D46" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="E46" s="18" t="s">
+      <c r="E46" s="21" t="s">
         <v>90</v>
       </c>
       <c r="F46" s="8" t="s">
@@ -1794,7 +1705,7 @@
       <c r="D47" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E47" s="24"/>
+      <c r="E47" s="22"/>
       <c r="F47" s="4" t="s">
         <v>91</v>
       </c>
@@ -1806,7 +1717,7 @@
       <c r="D48" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="E48" s="19"/>
+      <c r="E48" s="23"/>
       <c r="F48" s="4" t="s">
         <v>92</v>
       </c>
@@ -1815,12 +1726,12 @@
       </c>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D49" s="25" t="s">
+      <c r="D49" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="27"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="29"/>
     </row>
     <row r="50" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D50" s="5" t="s">
@@ -1847,18 +1758,18 @@
       </c>
     </row>
     <row r="52" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D52" s="23" t="s">
+      <c r="D52" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="E52" s="23"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="23"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
     </row>
     <row r="53" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D53" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="E53" s="20" t="s">
+      <c r="E53" s="16" t="s">
         <v>123</v>
       </c>
       <c r="F53" s="10" t="s">
@@ -1870,7 +1781,7 @@
       <c r="D54" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="E54" s="21"/>
+      <c r="E54" s="17"/>
       <c r="F54" s="10" t="s">
         <v>125</v>
       </c>
@@ -1882,7 +1793,7 @@
       <c r="D55" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="E55" s="21"/>
+      <c r="E55" s="17"/>
       <c r="F55" s="10" t="s">
         <v>126</v>
       </c>
@@ -1894,7 +1805,7 @@
       <c r="D56" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="E56" s="21"/>
+      <c r="E56" s="17"/>
       <c r="F56" s="10" t="s">
         <v>129</v>
       </c>
@@ -1906,9 +1817,9 @@
       <c r="D57" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="E57" s="21"/>
+      <c r="E57" s="17"/>
       <c r="F57" s="11" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="G57" s="10" t="s">
         <v>136</v>
@@ -1918,9 +1829,9 @@
       <c r="D58" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E58" s="22"/>
+      <c r="E58" s="18"/>
       <c r="F58" s="11" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="G58" s="11" t="s">
         <v>135</v>
@@ -1930,7 +1841,7 @@
       <c r="D59" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="E59" s="20" t="s">
+      <c r="E59" s="16" t="s">
         <v>137</v>
       </c>
       <c r="F59" s="10" t="s">
@@ -1944,7 +1855,7 @@
       <c r="D60" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E60" s="21"/>
+      <c r="E60" s="17"/>
       <c r="F60" s="10" t="s">
         <v>139</v>
       </c>
@@ -1956,7 +1867,7 @@
       <c r="D61" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="E61" s="22"/>
+      <c r="E61" s="18"/>
       <c r="F61" s="11" t="s">
         <v>140</v>
       </c>
@@ -1968,7 +1879,7 @@
       <c r="D62" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="E62" s="20" t="s">
+      <c r="E62" s="16" t="s">
         <v>144</v>
       </c>
       <c r="F62" s="10" t="s">
@@ -1982,7 +1893,7 @@
       <c r="D63" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="E63" s="21"/>
+      <c r="E63" s="17"/>
       <c r="F63" s="10" t="s">
         <v>145</v>
       </c>
@@ -1994,7 +1905,7 @@
       <c r="D64" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="E64" s="22"/>
+      <c r="E64" s="18"/>
       <c r="F64" s="10" t="s">
         <v>146</v>
       </c>
@@ -2006,11 +1917,11 @@
       <c r="D65" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="E65" s="20" t="s">
-        <v>191</v>
+      <c r="E65" s="16" t="s">
+        <v>181</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="G65" s="10" t="s">
         <v>170</v>
@@ -2018,11 +1929,11 @@
     </row>
     <row r="66" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D66" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="E66" s="21"/>
+        <v>173</v>
+      </c>
+      <c r="E66" s="17"/>
       <c r="F66" s="10" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="G66" s="10" t="s">
         <v>171</v>
@@ -2030,211 +1941,119 @@
     </row>
     <row r="67" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D67" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="E67" s="22"/>
+        <v>174</v>
+      </c>
+      <c r="E67" s="18"/>
       <c r="F67" s="10" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="G67" s="10" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="68" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D68" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="E68" s="20" t="s">
+      <c r="D68" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="E68" s="16" t="s">
         <v>163</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="69" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D69" s="21"/>
-      <c r="E69" s="21"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="17"/>
       <c r="F69" s="11" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
     </row>
     <row r="70" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D70" s="21"/>
-      <c r="E70" s="21"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
       <c r="F70" s="11" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="4:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="D71" s="21"/>
-      <c r="E71" s="21"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="17"/>
       <c r="F71" s="11" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="72" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D72" s="22"/>
-      <c r="E72" s="22"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="18"/>
       <c r="F72" s="11" t="s">
         <v>164</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
     </row>
     <row r="73" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D73" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="E73" s="23"/>
-      <c r="F73" s="23"/>
-      <c r="G73" s="23"/>
-    </row>
-    <row r="74" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D74" s="42" t="s">
+      <c r="D73" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19"/>
+      <c r="G73" s="19"/>
+    </row>
+    <row r="74" spans="4:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D74" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="E74" s="12"/>
+      <c r="F74" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="G74" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="E74" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="F74" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="G74" s="14" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="75" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D75" s="40"/>
-      <c r="E75" s="39"/>
-      <c r="F75" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="G75" s="14" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="76" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D76" s="41"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="G76" s="14" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="77" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D77" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="E77" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="F77" s="38" t="s">
-        <v>211</v>
-      </c>
-      <c r="G77" s="14" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="78" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D78" s="39"/>
-      <c r="E78" s="39"/>
-      <c r="F78" s="38" t="s">
-        <v>212</v>
-      </c>
-      <c r="G78" s="13" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="79" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D79" s="39"/>
-      <c r="E79" s="39"/>
-      <c r="F79" s="38" t="s">
-        <v>213</v>
-      </c>
-      <c r="G79" s="13" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="80" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D80" s="39"/>
-      <c r="E80" s="39"/>
-      <c r="F80" s="38" t="s">
-        <v>214</v>
-      </c>
-      <c r="G80" s="13" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="81" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D81" s="17"/>
-      <c r="E81" s="17"/>
-      <c r="F81" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="G81" s="13" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="82" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D82" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="E82" s="12"/>
-      <c r="F82" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="G82" s="14" t="s">
-        <v>190</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="D68:D72"/>
-    <mergeCell ref="E77:E81"/>
-    <mergeCell ref="D77:D81"/>
-    <mergeCell ref="E74:E76"/>
-    <mergeCell ref="D74:D76"/>
+  <mergeCells count="27">
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="E68:E72"/>
+    <mergeCell ref="D73:G73"/>
+    <mergeCell ref="D52:G52"/>
+    <mergeCell ref="E53:E58"/>
+    <mergeCell ref="E42:E45"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E59:E61"/>
+    <mergeCell ref="E62:E64"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E17:E22"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="E35:E37"/>
     <mergeCell ref="D6:G6"/>
     <mergeCell ref="D7:G7"/>
     <mergeCell ref="D8:D10"/>
     <mergeCell ref="D16:G16"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E8:E11"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E17:E22"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="E42:E45"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E59:E61"/>
-    <mergeCell ref="E62:E64"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="E68:E72"/>
-    <mergeCell ref="D73:G73"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="E53:E58"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D68:D72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>